<commit_message>
added data, tried (and failed) to scale xsec axes correctly
</commit_message>
<xml_diff>
--- a/notebooks/prototype_notebooks/Chloe_Gottesacker/GK_xsec_data_all.xlsx
+++ b/notebooks/prototype_notebooks/Chloe_Gottesacker/GK_xsec_data_all.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chloe\Documents\GitHub\gempy\notebooks\prototype_notebooks\Chloe_Gottesacker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D2891D-36BF-46C3-87AE-0BB9FD0D0A5A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C03CBAD-9F6C-46DE-AFF8-B7295CA07BD4}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="199">
   <si>
     <t>ID</t>
   </si>
@@ -622,48 +622,6 @@
   </si>
   <si>
     <t>AB-13c</t>
-  </si>
-  <si>
-    <t>585,600.969  5,249,606.841</t>
-  </si>
-  <si>
-    <t>585,452.802  5,249,413.695</t>
-  </si>
-  <si>
-    <t>585,452.802  5,249,413.696</t>
-  </si>
-  <si>
-    <t>585,386.656  5,249,331.674</t>
-  </si>
-  <si>
-    <t>585,208.062  5,249,098.840</t>
-  </si>
-  <si>
-    <t>585,107.520  5,248,973.162</t>
-  </si>
-  <si>
-    <t>584,992.558  5,248,822.217</t>
-  </si>
-  <si>
-    <t>584,844.391  5,248,634.363</t>
-  </si>
-  <si>
-    <t>584,680.349  5,248,421.373</t>
-  </si>
-  <si>
-    <t>584,566.578  5,248,274.529</t>
-  </si>
-  <si>
-    <t>584,434.286  5,248,107.841</t>
-  </si>
-  <si>
-    <t>584,264.953  5,247,886.913</t>
-  </si>
-  <si>
-    <t>583,991.770  5,247,537.001</t>
-  </si>
-  <si>
-    <t>583,922.978  5,247,453.657</t>
   </si>
   <si>
     <t>CT98</t>
@@ -1154,7 +1112,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1162,6 +1120,7 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1521,8 +1480,8 @@
   <dimension ref="A1:M191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C150" sqref="C150:D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -7886,10 +7845,10 @@
       <c r="B150" t="s">
         <v>169</v>
       </c>
-      <c r="C150" s="1">
+      <c r="C150" s="7">
         <v>586424.94700000004</v>
       </c>
-      <c r="D150" s="1">
+      <c r="D150" s="7">
         <v>5245283.4280000003</v>
       </c>
       <c r="E150" t="s">
@@ -7928,10 +7887,10 @@
       <c r="B151" t="s">
         <v>171</v>
       </c>
-      <c r="C151" s="1">
+      <c r="C151" s="7">
         <v>586583.16799999995</v>
       </c>
-      <c r="D151" s="1">
+      <c r="D151" s="7">
         <v>5245906.2580000004</v>
       </c>
       <c r="E151" t="s">
@@ -7970,10 +7929,10 @@
       <c r="B152" t="s">
         <v>172</v>
       </c>
-      <c r="C152" s="1">
+      <c r="C152" s="7">
         <v>586134.43400000001</v>
       </c>
-      <c r="D152" s="1">
+      <c r="D152" s="7">
         <v>5245360.1569999997</v>
       </c>
       <c r="E152" t="s">
@@ -8012,8 +7971,11 @@
       <c r="B153" t="s">
         <v>176</v>
       </c>
-      <c r="C153" t="s">
-        <v>198</v>
+      <c r="C153" s="7">
+        <v>585600.96900000004</v>
+      </c>
+      <c r="D153" s="7">
+        <v>5249606.841</v>
       </c>
       <c r="E153">
         <v>1150</v>
@@ -8022,14 +7984,14 @@
         <v>1100</v>
       </c>
       <c r="G153">
-        <f>E153-F153</f>
+        <f t="shared" ref="G153:G190" si="9">E153-F153</f>
         <v>50</v>
       </c>
       <c r="H153">
         <v>1225</v>
       </c>
       <c r="I153">
-        <f>H153-G153</f>
+        <f t="shared" ref="I153:I168" si="10">H153-G153</f>
         <v>1175</v>
       </c>
       <c r="J153" t="s">
@@ -8042,7 +8004,7 @@
         <v>177</v>
       </c>
       <c r="M153">
-        <f>H153-E153</f>
+        <f t="shared" ref="M153:M190" si="11">H153-E153</f>
         <v>75</v>
       </c>
     </row>
@@ -8053,8 +8015,11 @@
       <c r="B154" t="s">
         <v>181</v>
       </c>
-      <c r="C154" t="s">
-        <v>202</v>
+      <c r="C154" s="7">
+        <v>585208.06200000003</v>
+      </c>
+      <c r="D154" s="7">
+        <v>5249098.84</v>
       </c>
       <c r="E154">
         <v>1410</v>
@@ -8063,14 +8028,14 @@
         <v>1305</v>
       </c>
       <c r="G154">
-        <f>E154-F154</f>
+        <f t="shared" si="9"/>
         <v>105</v>
       </c>
       <c r="H154">
         <v>1421</v>
       </c>
       <c r="I154">
-        <f>H154-G154</f>
+        <f t="shared" si="10"/>
         <v>1316</v>
       </c>
       <c r="J154" t="s">
@@ -8083,7 +8048,7 @@
         <v>177</v>
       </c>
       <c r="M154">
-        <f>H154-E154</f>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
@@ -8094,8 +8059,11 @@
       <c r="B155" t="s">
         <v>23</v>
       </c>
-      <c r="C155" t="s">
-        <v>207</v>
+      <c r="C155" s="7">
+        <v>584566.57799999998</v>
+      </c>
+      <c r="D155" s="7">
+        <v>5248274.5290000001</v>
       </c>
       <c r="E155">
         <v>1665</v>
@@ -8104,14 +8072,14 @@
         <v>1610</v>
       </c>
       <c r="G155">
-        <f>E155-F155</f>
+        <f t="shared" si="9"/>
         <v>55</v>
       </c>
       <c r="H155">
         <v>1650</v>
       </c>
       <c r="I155">
-        <f>H155-G155</f>
+        <f t="shared" si="10"/>
         <v>1595</v>
       </c>
       <c r="J155" t="s">
@@ -8124,7 +8092,7 @@
         <v>177</v>
       </c>
       <c r="M155">
-        <f>H155-E155</f>
+        <f t="shared" si="11"/>
         <v>-15</v>
       </c>
     </row>
@@ -8135,8 +8103,11 @@
       <c r="B156" t="s">
         <v>17</v>
       </c>
-      <c r="C156" t="s">
-        <v>208</v>
+      <c r="C156" s="7">
+        <v>584434.28599999996</v>
+      </c>
+      <c r="D156" s="7">
+        <v>5248107.841</v>
       </c>
       <c r="E156">
         <v>1725</v>
@@ -8145,14 +8116,14 @@
         <v>1260</v>
       </c>
       <c r="G156">
-        <f>E156-F156</f>
+        <f t="shared" si="9"/>
         <v>465</v>
       </c>
       <c r="H156">
         <v>1719</v>
       </c>
       <c r="I156">
-        <f>H156-G156</f>
+        <f t="shared" si="10"/>
         <v>1254</v>
       </c>
       <c r="J156" t="s">
@@ -8165,7 +8136,7 @@
         <v>177</v>
       </c>
       <c r="M156">
-        <f>H156-E156</f>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
     </row>
@@ -8176,8 +8147,11 @@
       <c r="B157" t="s">
         <v>195</v>
       </c>
-      <c r="C157" t="s">
-        <v>209</v>
+      <c r="C157" s="7">
+        <v>584264.95299999998</v>
+      </c>
+      <c r="D157" s="7">
+        <v>5247886.9129999997</v>
       </c>
       <c r="E157">
         <v>1800</v>
@@ -8186,14 +8160,14 @@
         <v>1800</v>
       </c>
       <c r="G157">
-        <f>E157-F157</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H157">
         <v>1813</v>
       </c>
       <c r="I157">
-        <f>H157-G157</f>
+        <f t="shared" si="10"/>
         <v>1813</v>
       </c>
       <c r="J157" t="s">
@@ -8206,7 +8180,7 @@
         <v>177</v>
       </c>
       <c r="M157">
-        <f>H157-E157</f>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
@@ -8217,8 +8191,11 @@
       <c r="B158" t="s">
         <v>19</v>
       </c>
-      <c r="C158" t="s">
-        <v>210</v>
+      <c r="C158" s="7">
+        <v>583991.77</v>
+      </c>
+      <c r="D158" s="7">
+        <v>5247537.0010000002</v>
       </c>
       <c r="E158">
         <v>1930</v>
@@ -8227,14 +8204,14 @@
         <v>1580</v>
       </c>
       <c r="G158">
-        <f>E158-F158</f>
+        <f t="shared" si="9"/>
         <v>350</v>
       </c>
       <c r="H158">
         <v>1929</v>
       </c>
       <c r="I158">
-        <f>H158-G158</f>
+        <f t="shared" si="10"/>
         <v>1579</v>
       </c>
       <c r="J158" t="s">
@@ -8247,7 +8224,7 @@
         <v>177</v>
       </c>
       <c r="M158">
-        <f>H158-E158</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
     </row>
@@ -8258,8 +8235,11 @@
       <c r="B159" t="s">
         <v>197</v>
       </c>
-      <c r="C159" t="s">
-        <v>211</v>
+      <c r="C159" s="7">
+        <v>583922.978</v>
+      </c>
+      <c r="D159" s="7">
+        <v>5247453.6569999997</v>
       </c>
       <c r="E159">
         <v>1880</v>
@@ -8268,14 +8248,14 @@
         <v>1580</v>
       </c>
       <c r="G159">
-        <f>E159-F159</f>
+        <f t="shared" si="9"/>
         <v>300</v>
       </c>
       <c r="H159">
         <v>1873</v>
       </c>
       <c r="I159">
-        <f>H159-G159</f>
+        <f t="shared" si="10"/>
         <v>1573</v>
       </c>
       <c r="J159" t="s">
@@ -8288,7 +8268,7 @@
         <v>177</v>
       </c>
       <c r="M159">
-        <f>H159-E159</f>
+        <f t="shared" si="11"/>
         <v>-7</v>
       </c>
     </row>
@@ -8299,8 +8279,11 @@
       <c r="B160" t="s">
         <v>180</v>
       </c>
-      <c r="C160" t="s">
-        <v>201</v>
+      <c r="C160" s="7">
+        <v>585386.65599999996</v>
+      </c>
+      <c r="D160" s="7">
+        <v>5249331.6739999996</v>
       </c>
       <c r="E160">
         <v>1400</v>
@@ -8309,14 +8292,14 @@
         <v>1025</v>
       </c>
       <c r="G160">
-        <f>E160-F160</f>
+        <f t="shared" si="9"/>
         <v>375</v>
       </c>
       <c r="H160">
         <v>1396</v>
       </c>
       <c r="I160">
-        <f>H160-G160</f>
+        <f t="shared" si="10"/>
         <v>1021</v>
       </c>
       <c r="J160" t="s">
@@ -8329,7 +8312,7 @@
         <v>177</v>
       </c>
       <c r="M160">
-        <f>H160-E160</f>
+        <f t="shared" si="11"/>
         <v>-4</v>
       </c>
     </row>
@@ -8340,8 +8323,11 @@
       <c r="B161" t="s">
         <v>184</v>
       </c>
-      <c r="C161" t="s">
-        <v>202</v>
+      <c r="C161" s="7">
+        <v>585208.06200000003</v>
+      </c>
+      <c r="D161" s="7">
+        <v>5249098.84</v>
       </c>
       <c r="E161">
         <v>1410</v>
@@ -8350,14 +8336,14 @@
         <v>960</v>
       </c>
       <c r="G161">
-        <f>E161-F161</f>
+        <f t="shared" si="9"/>
         <v>450</v>
       </c>
       <c r="H161">
         <v>1421</v>
       </c>
       <c r="I161">
-        <f>H161-G161</f>
+        <f t="shared" si="10"/>
         <v>971</v>
       </c>
       <c r="J161" t="s">
@@ -8370,7 +8356,7 @@
         <v>177</v>
       </c>
       <c r="M161">
-        <f>H161-E161</f>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
@@ -8381,8 +8367,11 @@
       <c r="B162" t="s">
         <v>185</v>
       </c>
-      <c r="C162" t="s">
-        <v>203</v>
+      <c r="C162" s="7">
+        <v>585107.52</v>
+      </c>
+      <c r="D162" s="7">
+        <v>5248973.1619999995</v>
       </c>
       <c r="E162">
         <v>1500</v>
@@ -8391,14 +8380,14 @@
         <v>970</v>
       </c>
       <c r="G162">
-        <f>E162-F162</f>
+        <f t="shared" si="9"/>
         <v>530</v>
       </c>
       <c r="H162">
         <v>1476</v>
       </c>
       <c r="I162">
-        <f>H162-G162</f>
+        <f t="shared" si="10"/>
         <v>946</v>
       </c>
       <c r="J162" t="s">
@@ -8411,7 +8400,7 @@
         <v>177</v>
       </c>
       <c r="M162">
-        <f>H162-E162</f>
+        <f t="shared" si="11"/>
         <v>-24</v>
       </c>
     </row>
@@ -8422,8 +8411,11 @@
       <c r="B163" t="s">
         <v>188</v>
       </c>
-      <c r="C163" t="s">
-        <v>204</v>
+      <c r="C163" s="7">
+        <v>584992.55799999996</v>
+      </c>
+      <c r="D163" s="7">
+        <v>5248822.2170000002</v>
       </c>
       <c r="E163">
         <v>1610</v>
@@ -8432,14 +8424,14 @@
         <v>1100</v>
       </c>
       <c r="G163">
-        <f>E163-F163</f>
+        <f t="shared" si="9"/>
         <v>510</v>
       </c>
       <c r="H163">
         <v>1599</v>
       </c>
       <c r="I163">
-        <f>H163-G163</f>
+        <f t="shared" si="10"/>
         <v>1089</v>
       </c>
       <c r="J163" t="s">
@@ -8452,7 +8444,7 @@
         <v>177</v>
       </c>
       <c r="M163">
-        <f>H163-E163</f>
+        <f t="shared" si="11"/>
         <v>-11</v>
       </c>
     </row>
@@ -8463,8 +8455,11 @@
       <c r="B164" t="s">
         <v>191</v>
       </c>
-      <c r="C164" t="s">
-        <v>205</v>
+      <c r="C164" s="7">
+        <v>584844.39099999995</v>
+      </c>
+      <c r="D164" s="7">
+        <v>5248634.3629999999</v>
       </c>
       <c r="E164">
         <v>1740</v>
@@ -8473,14 +8468,14 @@
         <v>1380</v>
       </c>
       <c r="G164">
-        <f>E164-F164</f>
+        <f t="shared" si="9"/>
         <v>360</v>
       </c>
       <c r="H164">
         <v>1767</v>
       </c>
       <c r="I164">
-        <f>H164-G164</f>
+        <f t="shared" si="10"/>
         <v>1407</v>
       </c>
       <c r="J164" t="s">
@@ -8493,7 +8488,7 @@
         <v>177</v>
       </c>
       <c r="M164">
-        <f>H164-E164</f>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
     </row>
@@ -8504,8 +8499,11 @@
       <c r="B165" t="s">
         <v>192</v>
       </c>
-      <c r="C165" t="s">
-        <v>206</v>
+      <c r="C165" s="7">
+        <v>584680.34900000005</v>
+      </c>
+      <c r="D165" s="7">
+        <v>5248421.3729999997</v>
       </c>
       <c r="E165">
         <v>1685</v>
@@ -8514,14 +8512,14 @@
         <v>1280</v>
       </c>
       <c r="G165">
-        <f>E165-F165</f>
+        <f t="shared" si="9"/>
         <v>405</v>
       </c>
       <c r="H165">
         <v>1683</v>
       </c>
       <c r="I165">
-        <f>H165-G165</f>
+        <f t="shared" si="10"/>
         <v>1278</v>
       </c>
       <c r="J165" t="s">
@@ -8534,7 +8532,7 @@
         <v>177</v>
       </c>
       <c r="M165">
-        <f>H165-E165</f>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
     </row>
@@ -8545,8 +8543,11 @@
       <c r="B166" t="s">
         <v>193</v>
       </c>
-      <c r="C166" t="s">
-        <v>207</v>
+      <c r="C166" s="7">
+        <v>584566.57799999998</v>
+      </c>
+      <c r="D166" s="7">
+        <v>5248274.5290000001</v>
       </c>
       <c r="E166">
         <v>1665</v>
@@ -8555,14 +8556,14 @@
         <v>1225</v>
       </c>
       <c r="G166">
-        <f>E166-F166</f>
+        <f t="shared" si="9"/>
         <v>440</v>
       </c>
       <c r="H166">
         <v>1650</v>
       </c>
       <c r="I166">
-        <f>H166-G166</f>
+        <f t="shared" si="10"/>
         <v>1210</v>
       </c>
       <c r="J166" t="s">
@@ -8575,7 +8576,7 @@
         <v>177</v>
       </c>
       <c r="M166">
-        <f>H166-E166</f>
+        <f t="shared" si="11"/>
         <v>-15</v>
       </c>
     </row>
@@ -8586,8 +8587,11 @@
       <c r="B167" t="s">
         <v>24</v>
       </c>
-      <c r="C167" t="s">
-        <v>208</v>
+      <c r="C167" s="7">
+        <v>584434.28599999996</v>
+      </c>
+      <c r="D167" s="7">
+        <v>5248107.841</v>
       </c>
       <c r="E167">
         <v>1725</v>
@@ -8596,14 +8600,14 @@
         <v>2120</v>
       </c>
       <c r="G167">
-        <f>E167-F167</f>
+        <f t="shared" si="9"/>
         <v>-395</v>
       </c>
       <c r="H167">
         <v>1719</v>
       </c>
       <c r="I167">
-        <f>H167-G167</f>
+        <f t="shared" si="10"/>
         <v>2114</v>
       </c>
       <c r="J167" t="s">
@@ -8616,7 +8620,7 @@
         <v>177</v>
       </c>
       <c r="M167">
-        <f>H167-E167</f>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
     </row>
@@ -8627,8 +8631,11 @@
       <c r="B168" t="s">
         <v>194</v>
       </c>
-      <c r="C168" t="s">
-        <v>209</v>
+      <c r="C168" s="7">
+        <v>584264.95299999998</v>
+      </c>
+      <c r="D168" s="7">
+        <v>5247886.9129999997</v>
       </c>
       <c r="E168">
         <v>1800</v>
@@ -8637,14 +8644,14 @@
         <v>2140</v>
       </c>
       <c r="G168">
-        <f>E168-F168</f>
+        <f t="shared" si="9"/>
         <v>-340</v>
       </c>
       <c r="H168">
         <v>1813</v>
       </c>
       <c r="I168">
-        <f>H168-G168</f>
+        <f t="shared" si="10"/>
         <v>2153</v>
       </c>
       <c r="J168" t="s">
@@ -8657,7 +8664,7 @@
         <v>177</v>
       </c>
       <c r="M168">
-        <f>H168-E168</f>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
@@ -8668,8 +8675,11 @@
       <c r="B169" t="s">
         <v>25</v>
       </c>
-      <c r="C169" t="s">
-        <v>210</v>
+      <c r="C169" s="7">
+        <v>583991.77</v>
+      </c>
+      <c r="D169" s="7">
+        <v>5247537.0010000002</v>
       </c>
       <c r="E169">
         <v>1930</v>
@@ -8678,7 +8688,7 @@
         <v>1930</v>
       </c>
       <c r="G169">
-        <f>E169-F169</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H169">
@@ -8698,7 +8708,7 @@
         <v>177</v>
       </c>
       <c r="M169">
-        <f>H169-E169</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
     </row>
@@ -8709,8 +8719,11 @@
       <c r="B170" t="s">
         <v>39</v>
       </c>
-      <c r="C170" t="s">
-        <v>211</v>
+      <c r="C170" s="7">
+        <v>583922.978</v>
+      </c>
+      <c r="D170" s="7">
+        <v>5247453.6569999997</v>
       </c>
       <c r="E170">
         <v>1880</v>
@@ -8719,7 +8732,7 @@
         <v>1880</v>
       </c>
       <c r="G170">
-        <f>E170-F170</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H170">
@@ -8739,7 +8752,7 @@
         <v>177</v>
       </c>
       <c r="M170">
-        <f>H170-E170</f>
+        <f t="shared" si="11"/>
         <v>-7</v>
       </c>
     </row>
@@ -8750,8 +8763,11 @@
       <c r="B171" t="s">
         <v>29</v>
       </c>
-      <c r="C171" t="s">
-        <v>199</v>
+      <c r="C171" s="7">
+        <v>585452.80200000003</v>
+      </c>
+      <c r="D171" s="7">
+        <v>5249413.6950000003</v>
       </c>
       <c r="E171">
         <v>1490</v>
@@ -8760,7 +8776,7 @@
         <v>1430</v>
       </c>
       <c r="G171">
-        <f>E171-F171</f>
+        <f t="shared" si="9"/>
         <v>60</v>
       </c>
       <c r="H171">
@@ -8780,7 +8796,7 @@
         <v>177</v>
       </c>
       <c r="M171">
-        <f>H171-E171</f>
+        <f t="shared" si="11"/>
         <v>-103</v>
       </c>
     </row>
@@ -8791,8 +8807,11 @@
       <c r="B172" t="s">
         <v>178</v>
       </c>
-      <c r="C172" t="s">
-        <v>201</v>
+      <c r="C172" s="7">
+        <v>585386.65599999996</v>
+      </c>
+      <c r="D172" s="7">
+        <v>5249331.6739999996</v>
       </c>
       <c r="E172">
         <v>1400</v>
@@ -8801,7 +8820,7 @@
         <v>1400</v>
       </c>
       <c r="G172">
-        <f>E172-F172</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H172">
@@ -8821,7 +8840,7 @@
         <v>177</v>
       </c>
       <c r="M172">
-        <f>H172-E172</f>
+        <f t="shared" si="11"/>
         <v>-4</v>
       </c>
     </row>
@@ -8832,8 +8851,11 @@
       <c r="B173" t="s">
         <v>182</v>
       </c>
-      <c r="C173" t="s">
-        <v>202</v>
+      <c r="C173" s="7">
+        <v>585208.06200000003</v>
+      </c>
+      <c r="D173" s="7">
+        <v>5249098.84</v>
       </c>
       <c r="E173">
         <v>1410</v>
@@ -8842,7 +8864,7 @@
         <v>1285</v>
       </c>
       <c r="G173">
-        <f>E173-F173</f>
+        <f t="shared" si="9"/>
         <v>125</v>
       </c>
       <c r="H173">
@@ -8862,7 +8884,7 @@
         <v>177</v>
       </c>
       <c r="M173">
-        <f>H173-E173</f>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
@@ -8873,8 +8895,11 @@
       <c r="B174" t="s">
         <v>32</v>
       </c>
-      <c r="C174" t="s">
-        <v>203</v>
+      <c r="C174" s="7">
+        <v>585107.52</v>
+      </c>
+      <c r="D174" s="7">
+        <v>5248973.1619999995</v>
       </c>
       <c r="E174">
         <v>1500</v>
@@ -8883,7 +8908,7 @@
         <v>1760</v>
       </c>
       <c r="G174">
-        <f>E174-F174</f>
+        <f t="shared" si="9"/>
         <v>-260</v>
       </c>
       <c r="H174">
@@ -8903,7 +8928,7 @@
         <v>177</v>
       </c>
       <c r="M174">
-        <f>H174-E174</f>
+        <f t="shared" si="11"/>
         <v>-24</v>
       </c>
     </row>
@@ -8914,8 +8939,11 @@
       <c r="B175" t="s">
         <v>186</v>
       </c>
-      <c r="C175" t="s">
-        <v>204</v>
+      <c r="C175" s="7">
+        <v>584992.55799999996</v>
+      </c>
+      <c r="D175" s="7">
+        <v>5248822.2170000002</v>
       </c>
       <c r="E175">
         <v>1610</v>
@@ -8924,7 +8952,7 @@
         <v>1800</v>
       </c>
       <c r="G175">
-        <f>E175-F175</f>
+        <f t="shared" si="9"/>
         <v>-190</v>
       </c>
       <c r="H175">
@@ -8944,7 +8972,7 @@
         <v>177</v>
       </c>
       <c r="M175">
-        <f>H175-E175</f>
+        <f t="shared" si="11"/>
         <v>-11</v>
       </c>
     </row>
@@ -8955,8 +8983,11 @@
       <c r="B176" t="s">
         <v>189</v>
       </c>
-      <c r="C176" t="s">
-        <v>205</v>
+      <c r="C176" s="7">
+        <v>584844.39099999995</v>
+      </c>
+      <c r="D176" s="7">
+        <v>5248634.3629999999</v>
       </c>
       <c r="E176">
         <v>1740</v>
@@ -8965,7 +8996,7 @@
         <v>1740</v>
       </c>
       <c r="G176">
-        <f>E176-F176</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H176">
@@ -8985,7 +9016,7 @@
         <v>177</v>
       </c>
       <c r="M176">
-        <f>H176-E176</f>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
     </row>
@@ -8996,8 +9027,11 @@
       <c r="B177" t="s">
         <v>35</v>
       </c>
-      <c r="C177" t="s">
-        <v>206</v>
+      <c r="C177" s="7">
+        <v>584680.34900000005</v>
+      </c>
+      <c r="D177" s="7">
+        <v>5248421.3729999997</v>
       </c>
       <c r="E177">
         <v>1685</v>
@@ -9006,14 +9040,14 @@
         <v>1665</v>
       </c>
       <c r="G177">
-        <f>E177-F177</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="H177">
         <v>1683</v>
       </c>
       <c r="I177">
-        <f>H177-G177</f>
+        <f t="shared" ref="I177:I190" si="12">H177-G177</f>
         <v>1663</v>
       </c>
       <c r="J177" t="s">
@@ -9026,7 +9060,7 @@
         <v>177</v>
       </c>
       <c r="M177">
-        <f>H177-E177</f>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
     </row>
@@ -9037,8 +9071,11 @@
       <c r="B178" t="s">
         <v>36</v>
       </c>
-      <c r="C178" t="s">
-        <v>207</v>
+      <c r="C178" s="7">
+        <v>584566.57799999998</v>
+      </c>
+      <c r="D178" s="7">
+        <v>5248274.5290000001</v>
       </c>
       <c r="E178">
         <v>1665</v>
@@ -9047,14 +9084,14 @@
         <v>1590</v>
       </c>
       <c r="G178">
-        <f>E178-F178</f>
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
       <c r="H178">
         <v>1650</v>
       </c>
       <c r="I178">
-        <f>H178-G178</f>
+        <f t="shared" si="12"/>
         <v>1575</v>
       </c>
       <c r="J178" t="s">
@@ -9067,7 +9104,7 @@
         <v>177</v>
       </c>
       <c r="M178">
-        <f>H178-E178</f>
+        <f t="shared" si="11"/>
         <v>-15</v>
       </c>
     </row>
@@ -9078,8 +9115,11 @@
       <c r="B179" t="s">
         <v>37</v>
       </c>
-      <c r="C179" t="s">
-        <v>208</v>
+      <c r="C179" s="7">
+        <v>584434.28599999996</v>
+      </c>
+      <c r="D179" s="7">
+        <v>5248107.841</v>
       </c>
       <c r="E179">
         <v>1725</v>
@@ -9088,14 +9128,14 @@
         <v>2015</v>
       </c>
       <c r="G179">
-        <f>E179-F179</f>
+        <f t="shared" si="9"/>
         <v>-290</v>
       </c>
       <c r="H179">
         <v>1719</v>
       </c>
       <c r="I179">
-        <f>H179-G179</f>
+        <f t="shared" si="12"/>
         <v>2009</v>
       </c>
       <c r="J179" t="s">
@@ -9108,7 +9148,7 @@
         <v>177</v>
       </c>
       <c r="M179">
-        <f>H179-E179</f>
+        <f t="shared" si="11"/>
         <v>-6</v>
       </c>
     </row>
@@ -9119,8 +9159,11 @@
       <c r="B180" t="s">
         <v>196</v>
       </c>
-      <c r="C180" t="s">
-        <v>209</v>
+      <c r="C180" s="7">
+        <v>584264.95299999998</v>
+      </c>
+      <c r="D180" s="7">
+        <v>5247886.9129999997</v>
       </c>
       <c r="E180">
         <v>1800</v>
@@ -9129,14 +9172,14 @@
         <v>2060</v>
       </c>
       <c r="G180">
-        <f>E180-F180</f>
+        <f t="shared" si="9"/>
         <v>-260</v>
       </c>
       <c r="H180">
         <v>1813</v>
       </c>
       <c r="I180">
-        <f>H180-G180</f>
+        <f t="shared" si="12"/>
         <v>2073</v>
       </c>
       <c r="J180" t="s">
@@ -9149,7 +9192,7 @@
         <v>177</v>
       </c>
       <c r="M180">
-        <f>H180-E180</f>
+        <f t="shared" si="11"/>
         <v>13</v>
       </c>
     </row>
@@ -9160,8 +9203,11 @@
       <c r="B181" t="s">
         <v>38</v>
       </c>
-      <c r="C181" t="s">
-        <v>210</v>
+      <c r="C181" s="7">
+        <v>583991.77</v>
+      </c>
+      <c r="D181" s="7">
+        <v>5247537.0010000002</v>
       </c>
       <c r="E181">
         <v>1930</v>
@@ -9170,14 +9216,14 @@
         <v>1840</v>
       </c>
       <c r="G181">
-        <f>E181-F181</f>
+        <f t="shared" si="9"/>
         <v>90</v>
       </c>
       <c r="H181">
         <v>1929</v>
       </c>
       <c r="I181">
-        <f>H181-G181</f>
+        <f t="shared" si="12"/>
         <v>1839</v>
       </c>
       <c r="J181" t="s">
@@ -9190,7 +9236,7 @@
         <v>177</v>
       </c>
       <c r="M181">
-        <f>H181-E181</f>
+        <f t="shared" si="11"/>
         <v>-1</v>
       </c>
     </row>
@@ -9201,8 +9247,11 @@
       <c r="B182" t="s">
         <v>20</v>
       </c>
-      <c r="C182" t="s">
-        <v>211</v>
+      <c r="C182" s="7">
+        <v>583922.978</v>
+      </c>
+      <c r="D182" s="7">
+        <v>5247453.6569999997</v>
       </c>
       <c r="E182">
         <v>1880</v>
@@ -9211,14 +9260,14 @@
         <v>1840</v>
       </c>
       <c r="G182">
-        <f>E182-F182</f>
+        <f t="shared" si="9"/>
         <v>40</v>
       </c>
       <c r="H182">
         <v>1873</v>
       </c>
       <c r="I182">
-        <f>H182-G182</f>
+        <f t="shared" si="12"/>
         <v>1833</v>
       </c>
       <c r="J182" t="s">
@@ -9231,7 +9280,7 @@
         <v>177</v>
       </c>
       <c r="M182">
-        <f>H182-E182</f>
+        <f t="shared" si="11"/>
         <v>-7</v>
       </c>
     </row>
@@ -9242,8 +9291,11 @@
       <c r="B183" t="s">
         <v>11</v>
       </c>
-      <c r="C183" t="s">
-        <v>200</v>
+      <c r="C183" s="7">
+        <v>585452.80200000003</v>
+      </c>
+      <c r="D183" s="7">
+        <v>5249413.6960000005</v>
       </c>
       <c r="E183">
         <v>1490</v>
@@ -9252,14 +9304,14 @@
         <v>1300</v>
       </c>
       <c r="G183">
-        <f>E183-F183</f>
+        <f t="shared" si="9"/>
         <v>190</v>
       </c>
       <c r="H183">
         <v>1387</v>
       </c>
       <c r="I183">
-        <f>H183-G183</f>
+        <f t="shared" si="12"/>
         <v>1197</v>
       </c>
       <c r="J183" t="s">
@@ -9272,7 +9324,7 @@
         <v>177</v>
       </c>
       <c r="M183">
-        <f>H183-E183</f>
+        <f t="shared" si="11"/>
         <v>-103</v>
       </c>
     </row>
@@ -9283,8 +9335,11 @@
       <c r="B184" t="s">
         <v>179</v>
       </c>
-      <c r="C184" t="s">
-        <v>201</v>
+      <c r="C184" s="7">
+        <v>585386.65599999996</v>
+      </c>
+      <c r="D184" s="7">
+        <v>5249331.6739999996</v>
       </c>
       <c r="E184">
         <v>1400</v>
@@ -9293,14 +9348,14 @@
         <v>1260</v>
       </c>
       <c r="G184">
-        <f>E184-F184</f>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H184">
         <v>1396</v>
       </c>
       <c r="I184">
-        <f>H184-G184</f>
+        <f t="shared" si="12"/>
         <v>1256</v>
       </c>
       <c r="J184" t="s">
@@ -9313,7 +9368,7 @@
         <v>177</v>
       </c>
       <c r="M184">
-        <f>H184-E184</f>
+        <f t="shared" si="11"/>
         <v>-4</v>
       </c>
     </row>
@@ -9324,8 +9379,11 @@
       <c r="B185" t="s">
         <v>183</v>
       </c>
-      <c r="C185" t="s">
-        <v>202</v>
+      <c r="C185" s="7">
+        <v>585208.06200000003</v>
+      </c>
+      <c r="D185" s="7">
+        <v>5249098.84</v>
       </c>
       <c r="E185">
         <v>1410</v>
@@ -9334,14 +9392,14 @@
         <v>1160</v>
       </c>
       <c r="G185">
-        <f>E185-F185</f>
+        <f t="shared" si="9"/>
         <v>250</v>
       </c>
       <c r="H185">
         <v>1421</v>
       </c>
       <c r="I185">
-        <f>H185-G185</f>
+        <f t="shared" si="12"/>
         <v>1171</v>
       </c>
       <c r="J185" t="s">
@@ -9354,7 +9412,7 @@
         <v>177</v>
       </c>
       <c r="M185">
-        <f>H185-E185</f>
+        <f t="shared" si="11"/>
         <v>11</v>
       </c>
     </row>
@@ -9365,8 +9423,11 @@
       <c r="B186" t="s">
         <v>14</v>
       </c>
-      <c r="C186" t="s">
-        <v>203</v>
+      <c r="C186" s="7">
+        <v>585107.52</v>
+      </c>
+      <c r="D186" s="7">
+        <v>5248973.1619999995</v>
       </c>
       <c r="E186">
         <v>1500</v>
@@ -9375,14 +9436,14 @@
         <v>1225</v>
       </c>
       <c r="G186">
-        <f>E186-F186</f>
+        <f t="shared" si="9"/>
         <v>275</v>
       </c>
       <c r="H186">
         <v>1476</v>
       </c>
       <c r="I186">
-        <f>H186-G186</f>
+        <f t="shared" si="12"/>
         <v>1201</v>
       </c>
       <c r="J186" t="s">
@@ -9395,7 +9456,7 @@
         <v>177</v>
       </c>
       <c r="M186">
-        <f>H186-E186</f>
+        <f t="shared" si="11"/>
         <v>-24</v>
       </c>
     </row>
@@ -9406,8 +9467,11 @@
       <c r="B187" t="s">
         <v>187</v>
       </c>
-      <c r="C187" t="s">
-        <v>204</v>
+      <c r="C187" s="7">
+        <v>584992.55799999996</v>
+      </c>
+      <c r="D187" s="7">
+        <v>5248822.2170000002</v>
       </c>
       <c r="E187">
         <v>1610</v>
@@ -9416,14 +9480,14 @@
         <v>1680</v>
       </c>
       <c r="G187">
-        <f>E187-F187</f>
+        <f t="shared" si="9"/>
         <v>-70</v>
       </c>
       <c r="H187">
         <v>1599</v>
       </c>
       <c r="I187">
-        <f>H187-G187</f>
+        <f t="shared" si="12"/>
         <v>1669</v>
       </c>
       <c r="J187" t="s">
@@ -9436,7 +9500,7 @@
         <v>177</v>
       </c>
       <c r="M187">
-        <f>H187-E187</f>
+        <f t="shared" si="11"/>
         <v>-11</v>
       </c>
     </row>
@@ -9447,8 +9511,11 @@
       <c r="B188" t="s">
         <v>190</v>
       </c>
-      <c r="C188" t="s">
-        <v>205</v>
+      <c r="C188" s="7">
+        <v>584844.39099999995</v>
+      </c>
+      <c r="D188" s="7">
+        <v>5248634.3629999999</v>
       </c>
       <c r="E188">
         <v>1740</v>
@@ -9457,14 +9524,14 @@
         <v>1600</v>
       </c>
       <c r="G188">
-        <f>E188-F188</f>
+        <f t="shared" si="9"/>
         <v>140</v>
       </c>
       <c r="H188">
         <v>1767</v>
       </c>
       <c r="I188">
-        <f>H188-G188</f>
+        <f t="shared" si="12"/>
         <v>1627</v>
       </c>
       <c r="J188" t="s">
@@ -9477,7 +9544,7 @@
         <v>177</v>
       </c>
       <c r="M188">
-        <f>H188-E188</f>
+        <f t="shared" si="11"/>
         <v>27</v>
       </c>
     </row>
@@ -9488,8 +9555,11 @@
       <c r="B189" t="s">
         <v>15</v>
       </c>
-      <c r="C189" t="s">
-        <v>206</v>
+      <c r="C189" s="7">
+        <v>584680.34900000005</v>
+      </c>
+      <c r="D189" s="7">
+        <v>5248421.3729999997</v>
       </c>
       <c r="E189">
         <v>1685</v>
@@ -9498,14 +9568,14 @@
         <v>1520</v>
       </c>
       <c r="G189">
-        <f>E189-F189</f>
+        <f t="shared" si="9"/>
         <v>165</v>
       </c>
       <c r="H189">
         <v>1683</v>
       </c>
       <c r="I189">
-        <f>H189-G189</f>
+        <f t="shared" si="12"/>
         <v>1518</v>
       </c>
       <c r="J189" t="s">
@@ -9518,7 +9588,7 @@
         <v>177</v>
       </c>
       <c r="M189">
-        <f>H189-E189</f>
+        <f t="shared" si="11"/>
         <v>-2</v>
       </c>
     </row>
@@ -9529,8 +9599,11 @@
       <c r="B190" t="s">
         <v>16</v>
       </c>
-      <c r="C190" t="s">
-        <v>207</v>
+      <c r="C190" s="7">
+        <v>584566.57799999998</v>
+      </c>
+      <c r="D190" s="7">
+        <v>5248274.5290000001</v>
       </c>
       <c r="E190">
         <v>1665</v>
@@ -9539,14 +9612,14 @@
         <v>1455</v>
       </c>
       <c r="G190">
-        <f>E190-F190</f>
+        <f t="shared" si="9"/>
         <v>210</v>
       </c>
       <c r="H190">
         <v>1650</v>
       </c>
       <c r="I190">
-        <f>H190-G190</f>
+        <f t="shared" si="12"/>
         <v>1440</v>
       </c>
       <c r="J190" t="s">
@@ -9559,13 +9632,13 @@
         <v>177</v>
       </c>
       <c r="M190">
-        <f>H190-E190</f>
+        <f t="shared" si="11"/>
         <v>-15</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.75">
       <c r="A191" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>